<commit_message>
xls2xml - adding field tvod_price
</commit_message>
<xml_diff>
--- a/xls2xml/tests_box/input_box_test.xlsx
+++ b/xls2xml/tests_box/input_box_test.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="referencias" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="categories" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="series" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="billingid" vbProcedure="false">referencias!$A$2:$A$12</definedName>
@@ -1888,17 +1889,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="44.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="68.13"/>
@@ -3477,7 +3478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3487,7 +3488,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.56"/>
@@ -5263,7 +5264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5273,7 +5274,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.56"/>
@@ -5422,4 +5423,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
xls2xml - adding trailers
</commit_message>
<xml_diff>
--- a/xls2xml/tests_box/input_box_test.xlsx
+++ b/xls2xml/tests_box/input_box_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="481">
   <si>
     <t xml:space="preserve">uuid_box</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t xml:space="preserve">subpasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preço</t>
   </si>
   <si>
     <t xml:space="preserve">198413c7-3d35-4c6d-9714-f80e92e9b7d0</t>
@@ -1895,57 +1898,59 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AV2" activeCellId="0" sqref="AV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="44.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="68.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="51.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="58.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="24.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="42.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="42.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="23.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="36.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="13.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="21.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="2" width="13.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="23.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="6.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="44.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="2" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="30.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="2" width="255.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="2" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="17.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="129.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="2" width="33.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="2" width="11.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="2" width="21.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="3" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="3" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="3" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="3" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="3" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="3" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="11.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="49" style="3" width="11.64"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="257" style="2" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1016" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="13.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="39" style="2" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="2" width="20.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="3" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="3" width="13.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="3" width="13.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="3" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="3" width="20.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="3" width="11.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="48" style="3" width="11.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="257" style="2" width="11.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="1016" style="1" width="11.8"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2095,9 @@
       <c r="AU1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="7"/>
+      <c r="AV1" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="AW1" s="8"/>
       <c r="AX1" s="8"/>
       <c r="AY1" s="8"/>
@@ -2312,43 +2319,43 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="V2" s="12" t="n">
         <v>2016</v>
@@ -2360,25 +2367,25 @@
         <v>9</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Z2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AH2" s="13" t="n">
         <v>0.0164467592592593</v>
@@ -2390,13 +2397,16 @@
         <v>46387</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="AV2" s="3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="1047510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3488,7 +3498,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.56"/>
@@ -3511,1745 +3521,1745 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J1" s="16"/>
       <c r="K1" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="17" t="n">
         <v>10</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K3" s="18" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" s="17" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C5" s="17" t="n">
         <v>14</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" s="17" t="n">
         <v>16</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="17" t="n">
         <v>18</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M13" s="16" t="s">
         <v>36</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q18" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q22" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q23" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q24" s="19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Q25" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q28" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q30" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q32" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Q33" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Q34" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Q36" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Q37" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q38" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Q39" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="Q40" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="Q41" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="Q42" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="Q43" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="Q44" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Q45" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Q46" s="19" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="Q47" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Q48" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Q49" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Q50" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Q51" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="Q52" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q53" s="19" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Q54" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="17" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="Q55" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="Q56" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="Q57" s="19" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="Q58" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Q59" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Q60" s="19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="Q61" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="17" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="Q62" s="19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Q63" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="17" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Q64" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Q65" s="19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="Q66" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="Q67" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="17" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q68" s="19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Q69" s="19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="Q70" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="Q71" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Q72" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="Q73" s="19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Q74" s="19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="Q75" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="Q76" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="17" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="Q77" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Q78" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Q79" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="17" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="Q80" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="17" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Q81" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Q82" s="19" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="17" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="Q83" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="17" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Q84" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="Q85" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="17" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Q86" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="17" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Q87" s="19" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="17" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="Q88" s="19" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="17" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="Q89" s="19" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="17" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="17" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="17" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="17" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="17" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="17" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="17" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="17" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="17" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="17" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="17" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="17" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="17" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="17" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="17" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="17" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="17" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="17" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="17" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="17" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="17" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="17" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="17" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="17" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="17" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="17" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="17" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="17" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="17" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E123" s="17" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="17" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="17" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="17" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="17" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="17" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="17" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="17" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="17" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E132" s="17" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="17" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E134" s="17" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="17" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E136" s="17" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="17" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="17" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E140" s="17" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E141" s="17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="17" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E143" s="17" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="17" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E145" s="17" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="17" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E147" s="17" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="17" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E149" s="17" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E150" s="17" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E151" s="17" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E152" s="17" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E153" s="17" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E154" s="17" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E155" s="17" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E156" s="17" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E157" s="17" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E158" s="17" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E159" s="17" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E160" s="17" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E161" s="17" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E162" s="17" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E163" s="17" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E164" s="17" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E165" s="17" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E166" s="17" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E167" s="17" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E168" s="17" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E169" s="17" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E170" s="17" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E171" s="17" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E172" s="17" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E173" s="17" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E174" s="17" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E175" s="17" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E176" s="17" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E177" s="17" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E178" s="17" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="17" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E180" s="17" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E181" s="17" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E182" s="17" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E183" s="17" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E184" s="17" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E185" s="17" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E186" s="17" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E187" s="17" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E188" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E189" s="17" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E190" s="17" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="17" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E192" s="17" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E193" s="17" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E194" s="17" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E195" s="17" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E196" s="17" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E197" s="17" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E198" s="17" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E199" s="17" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E200" s="17" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E201" s="17" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E202" s="17" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E203" s="17" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E204" s="17" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E205" s="17" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E206" s="17" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E207" s="17" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E208" s="17" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E209" s="17" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E210" s="17" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E211" s="17" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E212" s="17" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E213" s="17" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E214" s="17" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E215" s="17" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E216" s="17" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E217" s="17" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E218" s="17" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E219" s="17" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E220" s="17" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E221" s="17" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E222" s="17" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E223" s="17" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E224" s="17" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E225" s="17" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E226" s="17" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E227" s="17" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E228" s="17" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E229" s="17" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E230" s="17" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E231" s="17" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E232" s="17" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E233" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E234" s="17" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E235" s="17" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E236" s="17" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E237" s="17" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E238" s="17" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E239" s="17" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E240" s="17" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E241" s="17" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E242" s="17" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E243" s="17" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E244" s="17" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E245" s="17" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E246" s="17" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E247" s="17" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -5274,7 +5284,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.56"/>
@@ -5286,132 +5296,132 @@
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>474</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>473</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -5432,11 +5442,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>